<commit_message>
Adicionei o Join Tabs
</commit_message>
<xml_diff>
--- a/Materiais auxliares/Files/Fill and aggragate.xlsx
+++ b/Materiais auxliares/Files/Fill and aggragate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiago.oliveira\OneDrive\Área de Trabalho\Developing\Formatter\Materiais auxliares\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiago.oliveira\OneDrive\Área de Trabalho\FormatterBR\Materiais auxliares\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B96974-4415-4DA5-8563-FC7972B17389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494003AA-C2CD-4DF0-895A-9FD7DF341E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="1350" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,35 +36,41 @@
     <t>bruno</t>
   </si>
   <si>
-    <t>Copia</t>
-  </si>
-  <si>
     <t>Rita</t>
   </si>
   <si>
     <t>Josias</t>
   </si>
   <si>
-    <t>tias</t>
-  </si>
-  <si>
-    <t>truta</t>
-  </si>
-  <si>
     <t>Nome</t>
   </si>
   <si>
     <t>XXXX</t>
+  </si>
+  <si>
+    <t>Exemple</t>
+  </si>
+  <si>
+    <t>Exemple2</t>
+  </si>
+  <si>
+    <t>Exemple3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -375,8 +381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,19 +394,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -417,22 +423,22 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E3" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E4" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E5" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -449,77 +455,78 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E11" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E12" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E13" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E14" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E15" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E16" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>